<commit_message>
Fix The Burning Kor reminder cards
</commit_message>
<xml_diff>
--- a/Nemesis Cards.xlsx
+++ b/Nemesis Cards.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAF827D0-FB11-495E-9236-D575983755E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E9E12-20A3-49E0-A82F-9D40575DD3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{469EDDF8-4014-40DC-8A9C-AE29F1C1DF6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Nemesis Cards" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$P$680</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Nemesis Cards'!$A$1:$P$680</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8164" uniqueCount="1524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8163" uniqueCount="1524">
   <si>
     <t># Name</t>
   </si>
@@ -4523,18 +4523,12 @@
     <t>Two spaces are adjacent if they are orthogonally touching.</t>
   </si>
   <si>
-    <t>- Once per turn, during any player's casting or main phase, that player may move their mage token to an adjacent space for free.#- During any player's casting or main phase, that player may discard a card to move their mage token to an adjacent space.#- M</t>
-  </si>
-  <si>
     <t>Southern Village</t>
   </si>
   <si>
     <t>The Burning Kor Player Aid - Damage Rules</t>
   </si>
   <si>
-    <t>- Players can only deal damage to embers that are orthogonally adjacent to their mage tokens.#- When a player deals damage to an ember, they can distribute that damage among any number of embers in spaces adjacent to their mage token.#- Embers are minions</t>
-  </si>
-  <si>
     <t>Ember Reminder</t>
   </si>
   <si>
@@ -4608,6 +4602,12 @@
   </si>
   <si>
     <t>Place three embers each on top different spaces adjacent to Gravehold.</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;- Once per turn, during any player's casting or main phase, that player may move their mage token to an adjacent space for free.#- During any player's casting or main phase, that player may discard a card to move their mage token to an adjacent space.#- Mage tokens cannot occupy the same space as embers or other mage tokens.#- Nothing can move onto Gravehold.#- Players can't move their mage tokens into any of the ignition points.</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;- Players can only deal damage to embers that are orthogonally adjacent to their mage tokens.#- When a player deals damage to an ember, they can distribute that damage among any number of embers in spaces adjacent to their mage token.#- Embers are minions and have 1 life.#- Reduce to 0 all damage dealt to The Burning Kor by players not on the edge of the board.</t>
   </si>
 </sst>
 </file>
@@ -5055,8 +5055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA3DCA3-0420-4130-9777-97966219C66E}">
   <dimension ref="A1:P680"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="J652" workbookViewId="0">
+      <selection activeCell="K671" sqref="K671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5210,9 +5210,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
@@ -35121,13 +35119,13 @@
         <v>45</v>
       </c>
       <c r="K669" s="1" t="s">
+        <v>1522</v>
+      </c>
+      <c r="L669" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M669" s="1" t="s">
         <v>1495</v>
-      </c>
-      <c r="L669" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M669" s="1" t="s">
-        <v>1496</v>
       </c>
       <c r="N669" s="1" t="s">
         <v>45</v>
@@ -35141,7 +35139,7 @@
     </row>
     <row r="670" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A670" s="1" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B670" s="1" t="s">
         <v>385</v>
@@ -35165,13 +35163,13 @@
         <v>45</v>
       </c>
       <c r="K670" s="1" t="s">
-        <v>1498</v>
+        <v>1523</v>
       </c>
       <c r="L670" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M670" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N670" s="1" t="s">
         <v>45</v>
@@ -35185,7 +35183,7 @@
     </row>
     <row r="671" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A671" s="1" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="B671" s="1" t="s">
         <v>385</v>
@@ -35209,13 +35207,13 @@
         <v>45</v>
       </c>
       <c r="K671" s="1" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="L671" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M671" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N671" s="1" t="s">
         <v>45</v>
@@ -35229,10 +35227,10 @@
     </row>
     <row r="672" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A672" s="1" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C672">
         <v>7</v>
@@ -35247,13 +35245,13 @@
         <v>45</v>
       </c>
       <c r="H672" s="1" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="I672" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J672" s="1" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="K672" s="1" t="s">
         <v>45</v>
@@ -35262,7 +35260,7 @@
         <v>45</v>
       </c>
       <c r="M672" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N672" s="1" t="s">
         <v>45</v>
@@ -35276,7 +35274,7 @@
     </row>
     <row r="673" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A673" s="1" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="B673" s="1" t="s">
         <v>39</v>
@@ -35300,13 +35298,13 @@
         <v>45</v>
       </c>
       <c r="K673" s="1" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="L673" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M673" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N673" s="1" t="s">
         <v>45</v>
@@ -35320,7 +35318,7 @@
     </row>
     <row r="674" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A674" s="1" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="B674" s="1" t="s">
         <v>18</v>
@@ -35338,7 +35336,7 @@
         <v>45</v>
       </c>
       <c r="H674" s="1" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="I674" s="1" t="s">
         <v>45</v>
@@ -35347,13 +35345,13 @@
         <v>45</v>
       </c>
       <c r="K674" s="1" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="L674" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M674" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N674" s="1" t="s">
         <v>45</v>
@@ -35367,10 +35365,10 @@
     </row>
     <row r="675" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A675" s="1" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C675">
         <v>12</v>
@@ -35385,13 +35383,13 @@
         <v>45</v>
       </c>
       <c r="H675" s="1" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="I675" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J675" s="1" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="K675" s="1" t="s">
         <v>45</v>
@@ -35400,7 +35398,7 @@
         <v>45</v>
       </c>
       <c r="M675" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N675" s="1" t="s">
         <v>45</v>
@@ -35414,7 +35412,7 @@
     </row>
     <row r="676" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A676" s="1" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="B676" s="1" t="s">
         <v>39</v>
@@ -35438,13 +35436,13 @@
         <v>45</v>
       </c>
       <c r="K676" s="1" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="L676" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M676" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N676" s="1" t="s">
         <v>45</v>
@@ -35458,7 +35456,7 @@
     </row>
     <row r="677" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A677" s="1" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="B677" s="1" t="s">
         <v>18</v>
@@ -35476,7 +35474,7 @@
         <v>45</v>
       </c>
       <c r="H677" s="1" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="I677" s="1" t="s">
         <v>45</v>
@@ -35491,7 +35489,7 @@
         <v>45</v>
       </c>
       <c r="M677" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N677" s="1" t="s">
         <v>45</v>
@@ -35505,10 +35503,10 @@
     </row>
     <row r="678" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A678" s="1" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C678">
         <v>23</v>
@@ -35523,13 +35521,13 @@
         <v>45</v>
       </c>
       <c r="H678" s="1" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="I678" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J678" s="1" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="K678" s="1" t="s">
         <v>45</v>
@@ -35538,7 +35536,7 @@
         <v>45</v>
       </c>
       <c r="M678" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N678" s="1" t="s">
         <v>45</v>
@@ -35552,7 +35550,7 @@
     </row>
     <row r="679" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A679" s="1" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="B679" s="1" t="s">
         <v>39</v>
@@ -35576,13 +35574,13 @@
         <v>45</v>
       </c>
       <c r="K679" s="1" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="L679" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M679" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N679" s="1" t="s">
         <v>45</v>
@@ -35596,7 +35594,7 @@
     </row>
     <row r="680" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A680" s="1" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="B680" s="1" t="s">
         <v>18</v>
@@ -35623,13 +35621,13 @@
         <v>45</v>
       </c>
       <c r="K680" s="1" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="L680" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M680" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="N680" s="1" t="s">
         <v>45</v>

</xml_diff>